<commit_message>
Atualizando a tabela de classificacao
</commit_message>
<xml_diff>
--- a/dataset/classificacao_casa_23.xlsx
+++ b/dataset/classificacao_casa_23.xlsx
@@ -75,13 +75,13 @@
     <t>5º</t>
   </si>
   <si>
-    <t>Bragantino</t>
+    <t>Red Bull Bragantino</t>
   </si>
   <si>
     <t>6º</t>
   </si>
   <si>
-    <t>Athletico-PR</t>
+    <t>Athletico - PR</t>
   </si>
   <si>
     <t>7º</t>
@@ -117,7 +117,7 @@
     <t>12º</t>
   </si>
   <si>
-    <t>Atlético-MG</t>
+    <t>Atlético - MG</t>
   </si>
   <si>
     <t>13º</t>
@@ -147,7 +147,7 @@
     <t>17º</t>
   </si>
   <si>
-    <t>América-MG</t>
+    <t>América - MG</t>
   </si>
   <si>
     <t>18º</t>
@@ -216,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border/>
     <border>
       <left style="thin">
@@ -298,11 +298,25 @@
         <color rgb="FFE4E4E4"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFEEEEEE"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFEEEEEE"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFEEEEEE"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -338,6 +352,9 @@
     </xf>
     <xf borderId="7" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="8" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -723,7 +740,7 @@
       <c r="A6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="7">

</xml_diff>